<commit_message>
termino generacion de cruces CRM - PRECIO
</commit_message>
<xml_diff>
--- a/CRM Comercial 2 Compass.xlsx
+++ b/CRM Comercial 2 Compass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo PL\Desktop\Automatizaciones\Automatizacione-EMP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0257FAEF-4B67-45D7-BDE9-5250F705A28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28634B2-E4A8-40A1-9728-9EEF2A88E6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4C01EB41-D205-410D-966C-732FE24FB6DB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4C01EB41-D205-410D-966C-732FE24FB6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="AGENDA" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2732" uniqueCount="504">
   <si>
     <t>Estado</t>
   </si>
@@ -1556,6 +1556,15 @@
   </si>
   <si>
     <t>17 KG</t>
+  </si>
+  <si>
+    <t>I22471</t>
+  </si>
+  <si>
+    <t>I23000</t>
+  </si>
+  <si>
+    <t>I25103</t>
   </si>
 </sst>
 </file>
@@ -1788,11 +1797,11 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -8748,7 +8757,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00C8ADBE-61B5-4C7E-9449-42411F58B4CB}" name="TablaDinámica3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00C8ADBE-61B5-4C7E-9449-42411F58B4CB}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="L3:N87" firstHeaderRow="1" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="23">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -9693,7 +9702,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{25DFF654-DFDA-4963-BE62-38176D9F93E8}" name="TablaDinámica2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{25DFF654-DFDA-4963-BE62-38176D9F93E8}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A21:D31" firstHeaderRow="1" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="23">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -11178,7 +11187,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{422E7DA4-F7ED-4D29-9F95-075C91A84093}" name="TablaDinámica4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{422E7DA4-F7ED-4D29-9F95-075C91A84093}" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A37:D55" firstHeaderRow="1" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="23">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -12696,7 +12705,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1053C9B9-40D6-4A13-8F0B-4E53CD89A103}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1053C9B9-40D6-4A13-8F0B-4E53CD89A103}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="23">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -14307,10 +14316,10 @@
   <dimension ref="A2:V238"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:AG1048576"/>
+      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -26305,7 +26314,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26314,22 +26323,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>474</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="3" spans="1:14" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -26386,25 +26395,28 @@
       <c r="D4" t="s">
         <v>487</v>
       </c>
+      <c r="F4" t="s">
+        <v>501</v>
+      </c>
       <c r="G4" t="s">
         <v>488</v>
       </c>
       <c r="H4" t="s">
         <v>489</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="36" t="s">
         <v>490</v>
       </c>
       <c r="J4" t="s">
         <v>491</v>
       </c>
-      <c r="L4" s="38">
+      <c r="L4" s="37">
         <v>3474.58</v>
       </c>
-      <c r="M4" s="38">
+      <c r="M4" s="37">
         <v>625.42399999999998</v>
       </c>
-      <c r="N4" s="38">
+      <c r="N4" s="37">
         <f>+M4+L4</f>
         <v>4100.0039999999999</v>
       </c>
@@ -26423,6 +26435,9 @@
       <c r="E5">
         <v>20601646367</v>
       </c>
+      <c r="F5" t="s">
+        <v>502</v>
+      </c>
       <c r="G5" t="s">
         <v>493</v>
       </c>
@@ -26435,15 +26450,15 @@
       <c r="J5" t="s">
         <v>496</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="37">
         <f>+N5/1.18</f>
         <v>14406.77966101695</v>
       </c>
-      <c r="M5" s="38">
+      <c r="M5" s="37">
         <f>+N5-L5</f>
         <v>2593.2203389830502</v>
       </c>
-      <c r="N5" s="38">
+      <c r="N5" s="37">
         <v>17000</v>
       </c>
     </row>
@@ -26461,6 +26476,9 @@
       <c r="E6">
         <v>20613618687</v>
       </c>
+      <c r="F6" t="s">
+        <v>503</v>
+      </c>
       <c r="G6" t="s">
         <v>498</v>
       </c>
@@ -26473,14 +26491,14 @@
       <c r="J6" t="s">
         <v>491</v>
       </c>
-      <c r="L6" s="38">
+      <c r="L6" s="37">
         <v>3950</v>
       </c>
-      <c r="M6" s="38">
+      <c r="M6" s="37">
         <f>+N6-L6</f>
         <v>711</v>
       </c>
-      <c r="N6" s="38">
+      <c r="N6" s="37">
         <v>4661</v>
       </c>
     </row>

</xml_diff>